<commit_message>
wbs insert 0903 1313
</commit_message>
<xml_diff>
--- a/000-要件定義/003-WBS.xlsx
+++ b/000-要件定義/003-WBS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\システム開発演習\000-要件定義\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F62ECB-6FF0-475F-8A7A-779810A11F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAFD378F-97E7-4666-A814-DC9BA350D193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1965,14 +1965,137 @@
     <xf numFmtId="49" fontId="2" fillId="10" borderId="83" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="177" fontId="3" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="5" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1980,11 +2103,77 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1992,281 +2181,92 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="5" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2976,7 +2976,7 @@
       <pane xSplit="6" ySplit="7" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" sqref="A1:A3"/>
+      <selection pane="bottomRight" activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="9.6"/>
@@ -2993,94 +2993,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" ht="10.5" customHeight="1">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="109" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="168" t="s">
+      <c r="B1" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="171" t="s">
+      <c r="C1" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="172"/>
-      <c r="E1" s="177" t="s">
+      <c r="D1" s="116"/>
+      <c r="E1" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="179" t="s">
+      <c r="F1" s="123" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="162">
+      <c r="G1" s="106">
         <v>45536</v>
       </c>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
-      <c r="P1" s="163"/>
-      <c r="Q1" s="163"/>
-      <c r="R1" s="163"/>
-      <c r="S1" s="163"/>
-      <c r="T1" s="163"/>
-      <c r="U1" s="163"/>
-      <c r="V1" s="163"/>
-      <c r="W1" s="163"/>
-      <c r="X1" s="163"/>
-      <c r="Y1" s="163"/>
-      <c r="Z1" s="163"/>
-      <c r="AA1" s="163"/>
-      <c r="AB1" s="163"/>
-      <c r="AC1" s="163"/>
-      <c r="AD1" s="163"/>
-      <c r="AE1" s="163"/>
-      <c r="AF1" s="163"/>
-      <c r="AG1" s="163"/>
-      <c r="AH1" s="163"/>
-      <c r="AI1" s="163"/>
-      <c r="AJ1" s="164"/>
-      <c r="AK1" s="162">
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="107"/>
+      <c r="L1" s="107"/>
+      <c r="M1" s="107"/>
+      <c r="N1" s="107"/>
+      <c r="O1" s="107"/>
+      <c r="P1" s="107"/>
+      <c r="Q1" s="107"/>
+      <c r="R1" s="107"/>
+      <c r="S1" s="107"/>
+      <c r="T1" s="107"/>
+      <c r="U1" s="107"/>
+      <c r="V1" s="107"/>
+      <c r="W1" s="107"/>
+      <c r="X1" s="107"/>
+      <c r="Y1" s="107"/>
+      <c r="Z1" s="107"/>
+      <c r="AA1" s="107"/>
+      <c r="AB1" s="107"/>
+      <c r="AC1" s="107"/>
+      <c r="AD1" s="107"/>
+      <c r="AE1" s="107"/>
+      <c r="AF1" s="107"/>
+      <c r="AG1" s="107"/>
+      <c r="AH1" s="107"/>
+      <c r="AI1" s="107"/>
+      <c r="AJ1" s="108"/>
+      <c r="AK1" s="106">
         <v>45566</v>
       </c>
-      <c r="AL1" s="163"/>
-      <c r="AM1" s="163"/>
-      <c r="AN1" s="163"/>
-      <c r="AO1" s="163"/>
-      <c r="AP1" s="163"/>
-      <c r="AQ1" s="163"/>
-      <c r="AR1" s="163"/>
-      <c r="AS1" s="163"/>
-      <c r="AT1" s="163"/>
-      <c r="AU1" s="163"/>
-      <c r="AV1" s="163"/>
-      <c r="AW1" s="163"/>
-      <c r="AX1" s="163"/>
-      <c r="AY1" s="163"/>
-      <c r="AZ1" s="163"/>
-      <c r="BA1" s="163"/>
-      <c r="BB1" s="163"/>
-      <c r="BC1" s="163"/>
-      <c r="BD1" s="163"/>
-      <c r="BE1" s="163"/>
-      <c r="BF1" s="163"/>
-      <c r="BG1" s="163"/>
-      <c r="BH1" s="163"/>
-      <c r="BI1" s="163"/>
-      <c r="BJ1" s="163"/>
-      <c r="BK1" s="163"/>
-      <c r="BL1" s="163"/>
-      <c r="BM1" s="163"/>
-      <c r="BN1" s="164"/>
+      <c r="AL1" s="107"/>
+      <c r="AM1" s="107"/>
+      <c r="AN1" s="107"/>
+      <c r="AO1" s="107"/>
+      <c r="AP1" s="107"/>
+      <c r="AQ1" s="107"/>
+      <c r="AR1" s="107"/>
+      <c r="AS1" s="107"/>
+      <c r="AT1" s="107"/>
+      <c r="AU1" s="107"/>
+      <c r="AV1" s="107"/>
+      <c r="AW1" s="107"/>
+      <c r="AX1" s="107"/>
+      <c r="AY1" s="107"/>
+      <c r="AZ1" s="107"/>
+      <c r="BA1" s="107"/>
+      <c r="BB1" s="107"/>
+      <c r="BC1" s="107"/>
+      <c r="BD1" s="107"/>
+      <c r="BE1" s="107"/>
+      <c r="BF1" s="107"/>
+      <c r="BG1" s="107"/>
+      <c r="BH1" s="107"/>
+      <c r="BI1" s="107"/>
+      <c r="BJ1" s="107"/>
+      <c r="BK1" s="107"/>
+      <c r="BL1" s="107"/>
+      <c r="BM1" s="107"/>
+      <c r="BN1" s="108"/>
     </row>
     <row r="2" spans="1:66" ht="10.5" customHeight="1">
-      <c r="A2" s="166"/>
-      <c r="B2" s="169"/>
-      <c r="C2" s="173"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="178"/>
-      <c r="F2" s="180"/>
+      <c r="A2" s="110"/>
+      <c r="B2" s="113"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="124"/>
       <c r="G2" s="46">
         <v>45537</v>
       </c>
@@ -3322,12 +3322,12 @@
       </c>
     </row>
     <row r="3" spans="1:66" s="2" customFormat="1" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A3" s="167"/>
-      <c r="B3" s="170"/>
-      <c r="C3" s="175"/>
-      <c r="D3" s="176"/>
-      <c r="E3" s="178"/>
-      <c r="F3" s="181"/>
+      <c r="A3" s="111"/>
+      <c r="B3" s="114"/>
+      <c r="C3" s="119"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="125"/>
       <c r="G3" s="48" t="s">
         <v>18</v>
       </c>
@@ -3510,20 +3510,20 @@
       </c>
     </row>
     <row r="4" spans="1:66" ht="13.5" customHeight="1">
-      <c r="A4" s="157">
+      <c r="A4" s="126">
         <v>1</v>
       </c>
       <c r="B4" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="158" t="s">
+      <c r="C4" s="128" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="159"/>
-      <c r="E4" s="124" t="s">
+      <c r="D4" s="129"/>
+      <c r="E4" s="132" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="160"/>
+      <c r="F4" s="134"/>
       <c r="G4" s="29"/>
       <c r="H4" s="61"/>
       <c r="I4" s="61"/>
@@ -3586,12 +3586,12 @@
       <c r="BN4" s="71"/>
     </row>
     <row r="5" spans="1:66" ht="13.5" customHeight="1">
-      <c r="A5" s="131"/>
+      <c r="A5" s="127"/>
       <c r="B5" s="34"/>
-      <c r="C5" s="111"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="122"/>
-      <c r="F5" s="161"/>
+      <c r="C5" s="130"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="133"/>
+      <c r="F5" s="135"/>
       <c r="G5" s="31"/>
       <c r="H5" s="62"/>
       <c r="I5" s="62"/>
@@ -3654,18 +3654,18 @@
       <c r="BN5" s="72"/>
     </row>
     <row r="6" spans="1:66" ht="13.5" customHeight="1">
-      <c r="A6" s="130">
+      <c r="A6" s="136">
         <v>2</v>
       </c>
       <c r="B6" s="34"/>
-      <c r="C6" s="128" t="s">
+      <c r="C6" s="143" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="129"/>
-      <c r="E6" s="125" t="s">
+      <c r="D6" s="144"/>
+      <c r="E6" s="147" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="155"/>
+      <c r="F6" s="148"/>
       <c r="G6" s="51"/>
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
@@ -3728,12 +3728,12 @@
       <c r="BN6" s="73"/>
     </row>
     <row r="7" spans="1:66" ht="13.5" customHeight="1">
-      <c r="A7" s="131"/>
+      <c r="A7" s="127"/>
       <c r="B7" s="34"/>
-      <c r="C7" s="132"/>
-      <c r="D7" s="133"/>
-      <c r="E7" s="124"/>
-      <c r="F7" s="156"/>
+      <c r="C7" s="145"/>
+      <c r="D7" s="146"/>
+      <c r="E7" s="132"/>
+      <c r="F7" s="149"/>
       <c r="G7" s="52"/>
       <c r="H7" s="31"/>
       <c r="I7" s="64"/>
@@ -3796,20 +3796,20 @@
       <c r="BN7" s="74"/>
     </row>
     <row r="8" spans="1:66" ht="13.5" customHeight="1">
-      <c r="A8" s="130">
+      <c r="A8" s="136">
         <v>3</v>
       </c>
       <c r="B8" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="113" t="s">
+      <c r="C8" s="176" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="114"/>
-      <c r="E8" s="124" t="s">
+      <c r="D8" s="177"/>
+      <c r="E8" s="132" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="127"/>
+      <c r="F8" s="181"/>
       <c r="G8" s="38"/>
       <c r="H8" s="65"/>
       <c r="I8" s="65"/>
@@ -3872,12 +3872,12 @@
       <c r="BN8" s="75"/>
     </row>
     <row r="9" spans="1:66" ht="13.5" customHeight="1">
-      <c r="A9" s="131"/>
+      <c r="A9" s="127"/>
       <c r="B9" s="36"/>
-      <c r="C9" s="115"/>
-      <c r="D9" s="116"/>
-      <c r="E9" s="122"/>
-      <c r="F9" s="107"/>
+      <c r="C9" s="139"/>
+      <c r="D9" s="140"/>
+      <c r="E9" s="133"/>
+      <c r="F9" s="166"/>
       <c r="G9" s="51"/>
       <c r="H9" s="63"/>
       <c r="I9" s="63"/>
@@ -3940,18 +3940,18 @@
       <c r="BN9" s="73"/>
     </row>
     <row r="10" spans="1:66" ht="13.5" customHeight="1">
-      <c r="A10" s="130">
+      <c r="A10" s="136">
         <v>4</v>
       </c>
       <c r="B10" s="36"/>
-      <c r="C10" s="117" t="s">
+      <c r="C10" s="137" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="118"/>
-      <c r="E10" s="125" t="s">
+      <c r="D10" s="138"/>
+      <c r="E10" s="147" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="106"/>
+      <c r="F10" s="165"/>
       <c r="G10" s="51"/>
       <c r="H10" s="63"/>
       <c r="I10" s="63"/>
@@ -3959,7 +3959,7 @@
       <c r="K10" s="63"/>
       <c r="L10" s="13"/>
       <c r="M10" s="19"/>
-      <c r="N10" s="63"/>
+      <c r="N10" s="30"/>
       <c r="O10" s="30"/>
       <c r="P10" s="63"/>
       <c r="Q10" s="63"/>
@@ -4014,12 +4014,12 @@
       <c r="BN10" s="73"/>
     </row>
     <row r="11" spans="1:66" ht="13.5" customHeight="1">
-      <c r="A11" s="131"/>
+      <c r="A11" s="127"/>
       <c r="B11" s="36"/>
-      <c r="C11" s="115"/>
-      <c r="D11" s="116"/>
-      <c r="E11" s="126"/>
-      <c r="F11" s="107"/>
+      <c r="C11" s="139"/>
+      <c r="D11" s="140"/>
+      <c r="E11" s="156"/>
+      <c r="F11" s="166"/>
       <c r="G11" s="51"/>
       <c r="H11" s="63"/>
       <c r="I11" s="63"/>
@@ -4082,18 +4082,18 @@
       <c r="BN11" s="73"/>
     </row>
     <row r="12" spans="1:66" ht="13.5" customHeight="1">
-      <c r="A12" s="130">
+      <c r="A12" s="136">
         <v>5</v>
       </c>
       <c r="B12" s="36"/>
-      <c r="C12" s="117" t="s">
+      <c r="C12" s="137" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="118"/>
-      <c r="E12" s="121" t="s">
+      <c r="D12" s="138"/>
+      <c r="E12" s="157" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="106"/>
+      <c r="F12" s="165"/>
       <c r="G12" s="51"/>
       <c r="H12" s="63"/>
       <c r="I12" s="63"/>
@@ -4156,12 +4156,12 @@
       <c r="BN12" s="73"/>
     </row>
     <row r="13" spans="1:66" ht="13.5" customHeight="1">
-      <c r="A13" s="131"/>
+      <c r="A13" s="127"/>
       <c r="B13" s="37"/>
-      <c r="C13" s="119"/>
-      <c r="D13" s="120"/>
-      <c r="E13" s="124"/>
-      <c r="F13" s="108"/>
+      <c r="C13" s="178"/>
+      <c r="D13" s="179"/>
+      <c r="E13" s="132"/>
+      <c r="F13" s="175"/>
       <c r="G13" s="53"/>
       <c r="H13" s="66"/>
       <c r="I13" s="66"/>
@@ -4224,20 +4224,20 @@
       <c r="BN13" s="97"/>
     </row>
     <row r="14" spans="1:66" ht="12" customHeight="1">
-      <c r="A14" s="130">
+      <c r="A14" s="136">
         <v>6</v>
       </c>
       <c r="B14" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="117" t="s">
+      <c r="C14" s="137" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="118"/>
-      <c r="E14" s="124" t="s">
+      <c r="D14" s="138"/>
+      <c r="E14" s="132" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="154"/>
+      <c r="F14" s="141"/>
       <c r="G14" s="50"/>
       <c r="H14" s="62"/>
       <c r="I14" s="62"/>
@@ -4247,16 +4247,16 @@
       <c r="M14" s="22"/>
       <c r="N14" s="67"/>
       <c r="O14" s="62"/>
-      <c r="P14" s="30"/>
+      <c r="P14" s="62"/>
       <c r="Q14" s="30"/>
       <c r="R14" s="30"/>
       <c r="S14" s="16"/>
       <c r="T14" s="22"/>
       <c r="U14" s="22"/>
       <c r="V14" s="30"/>
-      <c r="W14" s="6"/>
-      <c r="X14" s="6"/>
-      <c r="Y14" s="6"/>
+      <c r="W14" s="30"/>
+      <c r="X14" s="30"/>
+      <c r="Y14" s="30"/>
       <c r="Z14" s="16"/>
       <c r="AA14" s="22"/>
       <c r="AB14" s="22"/>
@@ -4300,12 +4300,12 @@
       <c r="BN14" s="72"/>
     </row>
     <row r="15" spans="1:66" ht="12" customHeight="1">
-      <c r="A15" s="131"/>
+      <c r="A15" s="127"/>
       <c r="B15" s="36"/>
-      <c r="C15" s="115"/>
-      <c r="D15" s="116"/>
-      <c r="E15" s="122"/>
-      <c r="F15" s="151"/>
+      <c r="C15" s="139"/>
+      <c r="D15" s="140"/>
+      <c r="E15" s="133"/>
+      <c r="F15" s="142"/>
       <c r="G15" s="50"/>
       <c r="H15" s="62"/>
       <c r="I15" s="62"/>
@@ -4368,15 +4368,15 @@
       <c r="BN15" s="72"/>
     </row>
     <row r="16" spans="1:66" ht="12" customHeight="1">
-      <c r="A16" s="130">
+      <c r="A16" s="136">
         <v>7</v>
       </c>
       <c r="B16" s="36"/>
-      <c r="C16" s="128" t="s">
+      <c r="C16" s="143" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="129"/>
-      <c r="E16" s="125" t="s">
+      <c r="D16" s="144"/>
+      <c r="E16" s="147" t="s">
         <v>50</v>
       </c>
       <c r="F16" s="152"/>
@@ -4390,15 +4390,15 @@
       <c r="N16" s="63"/>
       <c r="O16" s="63"/>
       <c r="P16" s="63"/>
-      <c r="Q16" s="63"/>
-      <c r="R16" s="63"/>
+      <c r="Q16" s="30"/>
+      <c r="R16" s="30"/>
       <c r="S16" s="13"/>
       <c r="T16" s="19"/>
       <c r="U16" s="19"/>
       <c r="V16" s="30"/>
       <c r="W16" s="30"/>
       <c r="X16" s="30"/>
-      <c r="Y16" s="9"/>
+      <c r="Y16" s="30"/>
       <c r="Z16" s="13"/>
       <c r="AA16" s="19"/>
       <c r="AB16" s="19"/>
@@ -4442,12 +4442,12 @@
       <c r="BN16" s="73"/>
     </row>
     <row r="17" spans="1:66" ht="12" customHeight="1">
-      <c r="A17" s="131"/>
+      <c r="A17" s="127"/>
       <c r="B17" s="36"/>
-      <c r="C17" s="109"/>
-      <c r="D17" s="110"/>
-      <c r="E17" s="124"/>
-      <c r="F17" s="154"/>
+      <c r="C17" s="150"/>
+      <c r="D17" s="151"/>
+      <c r="E17" s="132"/>
+      <c r="F17" s="141"/>
       <c r="G17" s="52"/>
       <c r="H17" s="64"/>
       <c r="I17" s="64"/>
@@ -4510,20 +4510,20 @@
       <c r="BN17" s="74"/>
     </row>
     <row r="18" spans="1:66" ht="12" customHeight="1">
-      <c r="A18" s="130">
+      <c r="A18" s="136">
         <v>8</v>
       </c>
       <c r="B18" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="137" t="s">
+      <c r="C18" s="153" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="138"/>
-      <c r="E18" s="124" t="s">
+      <c r="D18" s="154"/>
+      <c r="E18" s="132" t="s">
         <v>50</v>
       </c>
-      <c r="F18" s="150"/>
+      <c r="F18" s="155"/>
       <c r="G18" s="38"/>
       <c r="H18" s="65"/>
       <c r="I18" s="65"/>
@@ -4542,17 +4542,17 @@
       <c r="V18" s="6"/>
       <c r="W18" s="6"/>
       <c r="X18" s="6"/>
-      <c r="Y18" s="60"/>
+      <c r="Y18" s="6"/>
       <c r="Z18" s="15"/>
       <c r="AA18" s="21"/>
       <c r="AB18" s="21"/>
       <c r="AC18" s="60"/>
       <c r="AD18" s="60"/>
-      <c r="AE18" s="24"/>
-      <c r="AF18" s="24"/>
+      <c r="AE18" s="60"/>
+      <c r="AF18" s="60"/>
       <c r="AG18" s="15"/>
       <c r="AH18" s="22"/>
-      <c r="AI18" s="9"/>
+      <c r="AI18" s="60"/>
       <c r="AJ18" s="98"/>
       <c r="AK18" s="86"/>
       <c r="AL18" s="6"/>
@@ -4586,12 +4586,12 @@
       <c r="BN18" s="75"/>
     </row>
     <row r="19" spans="1:66" ht="12" customHeight="1">
-      <c r="A19" s="131"/>
+      <c r="A19" s="127"/>
       <c r="B19" s="36"/>
-      <c r="C19" s="111"/>
-      <c r="D19" s="112"/>
-      <c r="E19" s="122"/>
-      <c r="F19" s="151"/>
+      <c r="C19" s="130"/>
+      <c r="D19" s="131"/>
+      <c r="E19" s="133"/>
+      <c r="F19" s="142"/>
       <c r="G19" s="52"/>
       <c r="H19" s="64"/>
       <c r="I19" s="64"/>
@@ -4654,15 +4654,15 @@
       <c r="BN19" s="74"/>
     </row>
     <row r="20" spans="1:66" ht="12" customHeight="1">
-      <c r="A20" s="130">
+      <c r="A20" s="136">
         <v>9</v>
       </c>
       <c r="B20" s="36"/>
-      <c r="C20" s="128" t="s">
+      <c r="C20" s="143" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="129"/>
-      <c r="E20" s="125" t="s">
+      <c r="D20" s="144"/>
+      <c r="E20" s="147" t="s">
         <v>50</v>
       </c>
       <c r="F20" s="152"/>
@@ -4691,10 +4691,10 @@
       <c r="AC20" s="30"/>
       <c r="AD20" s="30"/>
       <c r="AE20" s="30"/>
-      <c r="AF20" s="24"/>
+      <c r="AF20" s="30"/>
       <c r="AG20" s="13"/>
       <c r="AH20" s="19"/>
-      <c r="AI20" s="24"/>
+      <c r="AI20" s="30"/>
       <c r="AJ20" s="73"/>
       <c r="AK20" s="85"/>
       <c r="AL20" s="24"/>
@@ -4728,12 +4728,12 @@
       <c r="BN20" s="73"/>
     </row>
     <row r="21" spans="1:66" ht="12" customHeight="1">
-      <c r="A21" s="131"/>
+      <c r="A21" s="127"/>
       <c r="B21" s="36"/>
-      <c r="C21" s="111"/>
-      <c r="D21" s="112"/>
-      <c r="E21" s="126"/>
-      <c r="F21" s="151"/>
+      <c r="C21" s="130"/>
+      <c r="D21" s="131"/>
+      <c r="E21" s="156"/>
+      <c r="F21" s="142"/>
       <c r="G21" s="52"/>
       <c r="H21" s="24"/>
       <c r="I21" s="24"/>
@@ -4796,15 +4796,15 @@
       <c r="BN21" s="74"/>
     </row>
     <row r="22" spans="1:66" ht="12" customHeight="1">
-      <c r="A22" s="130">
+      <c r="A22" s="136">
         <v>10</v>
       </c>
       <c r="B22" s="36"/>
-      <c r="C22" s="128" t="s">
+      <c r="C22" s="143" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="129"/>
-      <c r="E22" s="121" t="s">
+      <c r="D22" s="144"/>
+      <c r="E22" s="157" t="s">
         <v>50</v>
       </c>
       <c r="F22" s="152"/>
@@ -4830,13 +4830,13 @@
       <c r="Z22" s="25"/>
       <c r="AA22" s="26"/>
       <c r="AB22" s="26"/>
-      <c r="AC22" s="64"/>
-      <c r="AD22" s="64"/>
+      <c r="AC22" s="30"/>
+      <c r="AD22" s="30"/>
       <c r="AE22" s="30"/>
       <c r="AF22" s="30"/>
       <c r="AG22" s="25"/>
       <c r="AH22" s="26"/>
-      <c r="AI22" s="24"/>
+      <c r="AI22" s="30"/>
       <c r="AJ22" s="99"/>
       <c r="AK22" s="85"/>
       <c r="AL22" s="24"/>
@@ -4870,12 +4870,12 @@
       <c r="BN22" s="77"/>
     </row>
     <row r="23" spans="1:66" ht="12" customHeight="1">
-      <c r="A23" s="131"/>
+      <c r="A23" s="127"/>
       <c r="B23" s="37"/>
-      <c r="C23" s="132"/>
-      <c r="D23" s="133"/>
-      <c r="E23" s="124"/>
-      <c r="F23" s="153"/>
+      <c r="C23" s="145"/>
+      <c r="D23" s="146"/>
+      <c r="E23" s="132"/>
+      <c r="F23" s="158"/>
       <c r="G23" s="54"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
@@ -4938,20 +4938,20 @@
       <c r="BN23" s="78"/>
     </row>
     <row r="24" spans="1:66" ht="12" customHeight="1">
-      <c r="A24" s="130">
+      <c r="A24" s="136">
         <v>11</v>
       </c>
       <c r="B24" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="137" t="s">
+      <c r="C24" s="153" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="138"/>
-      <c r="E24" s="124" t="s">
+      <c r="D24" s="154"/>
+      <c r="E24" s="132" t="s">
         <v>50</v>
       </c>
-      <c r="F24" s="150"/>
+      <c r="F24" s="155"/>
       <c r="G24" s="38"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
@@ -4980,8 +4980,8 @@
       <c r="AF24" s="65"/>
       <c r="AG24" s="15"/>
       <c r="AH24" s="21"/>
-      <c r="AI24" s="30"/>
-      <c r="AJ24" s="80"/>
+      <c r="AI24" s="63"/>
+      <c r="AJ24" s="101"/>
       <c r="AK24" s="63"/>
       <c r="AL24" s="63"/>
       <c r="AM24" s="63"/>
@@ -5014,14 +5014,14 @@
       <c r="BN24" s="79"/>
     </row>
     <row r="25" spans="1:66" ht="12" customHeight="1">
-      <c r="A25" s="131"/>
+      <c r="A25" s="127"/>
       <c r="B25" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="111"/>
-      <c r="D25" s="112"/>
-      <c r="E25" s="126"/>
-      <c r="F25" s="151"/>
+      <c r="C25" s="130"/>
+      <c r="D25" s="131"/>
+      <c r="E25" s="156"/>
+      <c r="F25" s="142"/>
       <c r="G25" s="51"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
@@ -5084,18 +5084,18 @@
       <c r="BN25" s="80"/>
     </row>
     <row r="26" spans="1:66" ht="12" customHeight="1">
-      <c r="A26" s="130">
+      <c r="A26" s="136">
         <v>12</v>
       </c>
       <c r="B26" s="36"/>
-      <c r="C26" s="109" t="s">
+      <c r="C26" s="150" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="110"/>
-      <c r="E26" s="121" t="s">
+      <c r="D26" s="151"/>
+      <c r="E26" s="157" t="s">
         <v>50</v>
       </c>
-      <c r="F26" s="123"/>
+      <c r="F26" s="180"/>
       <c r="G26" s="50"/>
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
@@ -5124,10 +5124,10 @@
       <c r="AF26" s="62"/>
       <c r="AG26" s="16"/>
       <c r="AH26" s="22"/>
-      <c r="AI26" s="30"/>
+      <c r="AI26" s="63"/>
       <c r="AJ26" s="101"/>
       <c r="AK26" s="30"/>
-      <c r="AL26" s="63"/>
+      <c r="AL26" s="30"/>
       <c r="AM26" s="63"/>
       <c r="AN26" s="16"/>
       <c r="AO26" s="22"/>
@@ -5158,12 +5158,12 @@
       <c r="BN26" s="80"/>
     </row>
     <row r="27" spans="1:66" ht="12" customHeight="1">
-      <c r="A27" s="131"/>
+      <c r="A27" s="127"/>
       <c r="B27" s="36"/>
-      <c r="C27" s="111"/>
-      <c r="D27" s="112"/>
-      <c r="E27" s="122"/>
-      <c r="F27" s="107"/>
+      <c r="C27" s="130"/>
+      <c r="D27" s="131"/>
+      <c r="E27" s="133"/>
+      <c r="F27" s="166"/>
       <c r="G27" s="51"/>
       <c r="H27" s="95"/>
       <c r="I27" s="7"/>
@@ -5226,18 +5226,18 @@
       <c r="BN27" s="80"/>
     </row>
     <row r="28" spans="1:66" ht="12" customHeight="1">
-      <c r="A28" s="130">
+      <c r="A28" s="136">
         <v>13</v>
       </c>
       <c r="B28" s="36"/>
-      <c r="C28" s="128" t="s">
+      <c r="C28" s="143" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="129"/>
-      <c r="E28" s="125" t="s">
+      <c r="D28" s="144"/>
+      <c r="E28" s="147" t="s">
         <v>50</v>
       </c>
-      <c r="F28" s="106"/>
+      <c r="F28" s="165"/>
       <c r="G28" s="50"/>
       <c r="H28" s="9"/>
       <c r="I28" s="7"/>
@@ -5268,12 +5268,12 @@
       <c r="AH28" s="19"/>
       <c r="AI28" s="63"/>
       <c r="AJ28" s="80"/>
-      <c r="AK28" s="30"/>
+      <c r="AK28" s="91"/>
       <c r="AL28" s="30"/>
       <c r="AM28" s="30"/>
       <c r="AN28" s="13"/>
       <c r="AO28" s="19"/>
-      <c r="AP28" s="63"/>
+      <c r="AP28" s="30"/>
       <c r="AQ28" s="63"/>
       <c r="AR28" s="63"/>
       <c r="AS28" s="63"/>
@@ -5300,12 +5300,12 @@
       <c r="BN28" s="80"/>
     </row>
     <row r="29" spans="1:66" ht="12" customHeight="1">
-      <c r="A29" s="131"/>
+      <c r="A29" s="127"/>
       <c r="B29" s="36"/>
-      <c r="C29" s="111"/>
-      <c r="D29" s="112"/>
-      <c r="E29" s="122"/>
-      <c r="F29" s="107"/>
+      <c r="C29" s="130"/>
+      <c r="D29" s="131"/>
+      <c r="E29" s="133"/>
+      <c r="F29" s="166"/>
       <c r="G29" s="51"/>
       <c r="H29" s="7"/>
       <c r="I29" s="95"/>
@@ -5368,18 +5368,18 @@
       <c r="BN29" s="80"/>
     </row>
     <row r="30" spans="1:66" ht="12" customHeight="1">
-      <c r="A30" s="130">
+      <c r="A30" s="136">
         <v>14</v>
       </c>
       <c r="B30" s="36"/>
-      <c r="C30" s="128" t="s">
+      <c r="C30" s="143" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="129"/>
-      <c r="E30" s="125" t="s">
+      <c r="D30" s="144"/>
+      <c r="E30" s="147" t="s">
         <v>50</v>
       </c>
-      <c r="F30" s="106"/>
+      <c r="F30" s="165"/>
       <c r="G30" s="50"/>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
@@ -5412,12 +5412,12 @@
       <c r="AJ30" s="80"/>
       <c r="AK30" s="91"/>
       <c r="AL30" s="63"/>
-      <c r="AM30" s="30"/>
+      <c r="AM30" s="63"/>
       <c r="AN30" s="13"/>
       <c r="AO30" s="19"/>
       <c r="AP30" s="30"/>
       <c r="AQ30" s="30"/>
-      <c r="AR30" s="63"/>
+      <c r="AR30" s="30"/>
       <c r="AS30" s="63"/>
       <c r="AT30" s="63"/>
       <c r="AU30" s="13"/>
@@ -5442,12 +5442,12 @@
       <c r="BN30" s="80"/>
     </row>
     <row r="31" spans="1:66" ht="12" customHeight="1">
-      <c r="A31" s="131"/>
+      <c r="A31" s="127"/>
       <c r="B31" s="36"/>
-      <c r="C31" s="111"/>
-      <c r="D31" s="112"/>
-      <c r="E31" s="126"/>
-      <c r="F31" s="107"/>
+      <c r="C31" s="130"/>
+      <c r="D31" s="131"/>
+      <c r="E31" s="156"/>
+      <c r="F31" s="166"/>
       <c r="G31" s="51"/>
       <c r="H31" s="95"/>
       <c r="I31" s="7"/>
@@ -5510,18 +5510,18 @@
       <c r="BN31" s="80"/>
     </row>
     <row r="32" spans="1:66" ht="12" customHeight="1">
-      <c r="A32" s="130">
+      <c r="A32" s="136">
         <v>15</v>
       </c>
       <c r="B32" s="36"/>
-      <c r="C32" s="128" t="s">
+      <c r="C32" s="143" t="s">
         <v>47</v>
       </c>
-      <c r="D32" s="129"/>
-      <c r="E32" s="121" t="s">
+      <c r="D32" s="144"/>
+      <c r="E32" s="157" t="s">
         <v>50</v>
       </c>
-      <c r="F32" s="106"/>
+      <c r="F32" s="165"/>
       <c r="G32" s="52"/>
       <c r="H32" s="24"/>
       <c r="I32" s="24"/>
@@ -5558,10 +5558,10 @@
       <c r="AN32" s="25"/>
       <c r="AO32" s="26"/>
       <c r="AP32" s="64"/>
-      <c r="AQ32" s="30"/>
+      <c r="AQ32" s="64"/>
       <c r="AR32" s="30"/>
       <c r="AS32" s="30"/>
-      <c r="AT32" s="63"/>
+      <c r="AT32" s="30"/>
       <c r="AU32" s="25"/>
       <c r="AV32" s="26"/>
       <c r="AW32" s="26"/>
@@ -5584,12 +5584,12 @@
       <c r="BN32" s="77"/>
     </row>
     <row r="33" spans="1:67" ht="12" customHeight="1">
-      <c r="A33" s="131"/>
+      <c r="A33" s="127"/>
       <c r="B33" s="36"/>
-      <c r="C33" s="111"/>
-      <c r="D33" s="112"/>
-      <c r="E33" s="122"/>
-      <c r="F33" s="107"/>
+      <c r="C33" s="130"/>
+      <c r="D33" s="131"/>
+      <c r="E33" s="133"/>
+      <c r="F33" s="166"/>
       <c r="G33" s="52"/>
       <c r="H33" s="24"/>
       <c r="I33" s="24"/>
@@ -5652,18 +5652,18 @@
       <c r="BN33" s="77"/>
     </row>
     <row r="34" spans="1:67" ht="12" customHeight="1">
-      <c r="A34" s="130">
+      <c r="A34" s="136">
         <v>16</v>
       </c>
       <c r="B34" s="36"/>
-      <c r="C34" s="128" t="s">
+      <c r="C34" s="143" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="129"/>
-      <c r="E34" s="125" t="s">
+      <c r="D34" s="144"/>
+      <c r="E34" s="147" t="s">
         <v>50</v>
       </c>
-      <c r="F34" s="106"/>
+      <c r="F34" s="165"/>
       <c r="G34" s="52"/>
       <c r="H34" s="24"/>
       <c r="I34" s="24"/>
@@ -5702,14 +5702,14 @@
       <c r="AP34" s="64"/>
       <c r="AQ34" s="64"/>
       <c r="AR34" s="64"/>
-      <c r="AS34" s="30"/>
+      <c r="AS34" s="64"/>
       <c r="AT34" s="30"/>
       <c r="AU34" s="25"/>
       <c r="AV34" s="26"/>
       <c r="AW34" s="26"/>
       <c r="AX34" s="30"/>
       <c r="AY34" s="30"/>
-      <c r="AZ34" s="64"/>
+      <c r="AZ34" s="30"/>
       <c r="BA34" s="63"/>
       <c r="BB34" s="25"/>
       <c r="BC34" s="26"/>
@@ -5726,12 +5726,12 @@
       <c r="BN34" s="77"/>
     </row>
     <row r="35" spans="1:67" ht="12" customHeight="1">
-      <c r="A35" s="131"/>
+      <c r="A35" s="127"/>
       <c r="B35" s="36"/>
-      <c r="C35" s="111"/>
-      <c r="D35" s="112"/>
-      <c r="E35" s="122"/>
-      <c r="F35" s="107"/>
+      <c r="C35" s="130"/>
+      <c r="D35" s="131"/>
+      <c r="E35" s="133"/>
+      <c r="F35" s="166"/>
       <c r="G35" s="52"/>
       <c r="H35" s="24"/>
       <c r="I35" s="24"/>
@@ -5794,18 +5794,18 @@
       <c r="BN35" s="77"/>
     </row>
     <row r="36" spans="1:67" ht="12" customHeight="1">
-      <c r="A36" s="130">
+      <c r="A36" s="136">
         <v>17</v>
       </c>
       <c r="B36" s="36"/>
-      <c r="C36" s="128" t="s">
+      <c r="C36" s="143" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="129"/>
-      <c r="E36" s="125" t="s">
+      <c r="D36" s="144"/>
+      <c r="E36" s="147" t="s">
         <v>50</v>
       </c>
-      <c r="F36" s="106"/>
+      <c r="F36" s="165"/>
       <c r="G36" s="52"/>
       <c r="H36" s="24"/>
       <c r="I36" s="24"/>
@@ -5850,13 +5850,13 @@
       <c r="AV36" s="26"/>
       <c r="AW36" s="26"/>
       <c r="AX36" s="64"/>
-      <c r="AY36" s="30"/>
+      <c r="AY36" s="64"/>
       <c r="AZ36" s="30"/>
       <c r="BA36" s="30"/>
       <c r="BB36" s="25"/>
       <c r="BC36" s="26"/>
       <c r="BD36" s="30"/>
-      <c r="BE36" s="64"/>
+      <c r="BE36" s="30"/>
       <c r="BF36" s="64"/>
       <c r="BG36" s="64"/>
       <c r="BH36" s="64"/>
@@ -5868,12 +5868,12 @@
       <c r="BN36" s="77"/>
     </row>
     <row r="37" spans="1:67" ht="12" customHeight="1">
-      <c r="A37" s="131"/>
+      <c r="A37" s="127"/>
       <c r="B37" s="36"/>
-      <c r="C37" s="132"/>
-      <c r="D37" s="133"/>
-      <c r="E37" s="124"/>
-      <c r="F37" s="108"/>
+      <c r="C37" s="145"/>
+      <c r="D37" s="146"/>
+      <c r="E37" s="132"/>
+      <c r="F37" s="175"/>
       <c r="G37" s="52"/>
       <c r="H37" s="24"/>
       <c r="I37" s="24"/>
@@ -5936,20 +5936,20 @@
       <c r="BN37" s="77"/>
     </row>
     <row r="38" spans="1:67" ht="12" customHeight="1">
-      <c r="A38" s="130">
+      <c r="A38" s="136">
         <v>18</v>
       </c>
       <c r="B38" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="144" t="s">
+      <c r="C38" s="159" t="s">
         <v>34</v>
       </c>
-      <c r="D38" s="145"/>
-      <c r="E38" s="124" t="s">
+      <c r="D38" s="160"/>
+      <c r="E38" s="132" t="s">
         <v>50</v>
       </c>
-      <c r="F38" s="148"/>
+      <c r="F38" s="163"/>
       <c r="G38" s="38"/>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -6000,7 +6000,7 @@
       <c r="BB38" s="15"/>
       <c r="BC38" s="21"/>
       <c r="BD38" s="65"/>
-      <c r="BE38" s="60"/>
+      <c r="BE38" s="65"/>
       <c r="BF38" s="41"/>
       <c r="BG38" s="41"/>
       <c r="BH38" s="41"/>
@@ -6012,12 +6012,12 @@
       <c r="BN38" s="79"/>
     </row>
     <row r="39" spans="1:67" ht="12" customHeight="1">
-      <c r="A39" s="131"/>
+      <c r="A39" s="127"/>
       <c r="B39" s="34"/>
-      <c r="C39" s="146"/>
-      <c r="D39" s="147"/>
-      <c r="E39" s="124"/>
-      <c r="F39" s="149"/>
+      <c r="C39" s="161"/>
+      <c r="D39" s="162"/>
+      <c r="E39" s="132"/>
+      <c r="F39" s="164"/>
       <c r="G39" s="51"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -6080,20 +6080,20 @@
       <c r="BN39" s="78"/>
     </row>
     <row r="40" spans="1:67" ht="12" customHeight="1">
-      <c r="A40" s="130">
+      <c r="A40" s="136">
         <v>19</v>
       </c>
-      <c r="B40" s="135" t="s">
+      <c r="B40" s="168" t="s">
         <v>32</v>
       </c>
-      <c r="C40" s="137" t="s">
+      <c r="C40" s="153" t="s">
         <v>32</v>
       </c>
-      <c r="D40" s="138"/>
-      <c r="E40" s="122" t="s">
+      <c r="D40" s="154"/>
+      <c r="E40" s="133" t="s">
         <v>50</v>
       </c>
-      <c r="F40" s="142"/>
+      <c r="F40" s="173"/>
       <c r="G40" s="38"/>
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
@@ -6157,12 +6157,12 @@
       <c r="BO40" s="103"/>
     </row>
     <row r="41" spans="1:67" ht="12" customHeight="1" thickBot="1">
-      <c r="A41" s="134"/>
-      <c r="B41" s="136"/>
-      <c r="C41" s="139"/>
-      <c r="D41" s="140"/>
-      <c r="E41" s="141"/>
-      <c r="F41" s="143"/>
+      <c r="A41" s="167"/>
+      <c r="B41" s="169"/>
+      <c r="C41" s="170"/>
+      <c r="D41" s="171"/>
+      <c r="E41" s="172"/>
+      <c r="F41" s="174"/>
       <c r="G41" s="39"/>
       <c r="H41" s="11"/>
       <c r="I41" s="11"/>
@@ -6243,44 +6243,36 @@
     </row>
   </sheetData>
   <mergeCells count="84">
-    <mergeCell ref="AK1:BN1"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="C4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G1:AJ1"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="C14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="C6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="C16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="C20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="C22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="C26:D27"/>
+    <mergeCell ref="C8:D9"/>
+    <mergeCell ref="C10:D11"/>
+    <mergeCell ref="C12:D13"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="C30:D31"/>
+    <mergeCell ref="C28:D29"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="C36:D37"/>
+    <mergeCell ref="C34:D35"/>
+    <mergeCell ref="C32:D33"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F40:F41"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="C38:D39"/>
     <mergeCell ref="E38:E39"/>
@@ -6297,36 +6289,44 @@
     <mergeCell ref="F28:F29"/>
     <mergeCell ref="F30:F31"/>
     <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="C28:D29"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="C36:D37"/>
-    <mergeCell ref="C34:D35"/>
-    <mergeCell ref="C32:D33"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="C26:D27"/>
-    <mergeCell ref="C8:D9"/>
-    <mergeCell ref="C10:D11"/>
-    <mergeCell ref="C12:D13"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="C30:D31"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="C20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="C22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="C16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="C14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="C6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="C4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G1:AJ1"/>
+    <mergeCell ref="AK1:BN1"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <printOptions gridLinesSet="0"/>
@@ -6370,54 +6370,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="10.5" customHeight="1">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="109" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="168" t="s">
+      <c r="B1" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="171" t="s">
+      <c r="C1" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="172"/>
-      <c r="E1" s="177" t="s">
+      <c r="D1" s="116"/>
+      <c r="E1" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="179" t="s">
+      <c r="F1" s="123" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="162"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
-      <c r="P1" s="163"/>
-      <c r="Q1" s="163"/>
-      <c r="R1" s="163"/>
-      <c r="S1" s="163"/>
-      <c r="T1" s="163"/>
-      <c r="U1" s="163"/>
-      <c r="V1" s="163"/>
-      <c r="W1" s="163"/>
-      <c r="X1" s="163"/>
-      <c r="Y1" s="163"/>
-      <c r="Z1" s="163"/>
-      <c r="AA1" s="163"/>
-      <c r="AB1" s="163"/>
-      <c r="AC1" s="163"/>
-      <c r="AD1" s="164"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="107"/>
+      <c r="L1" s="107"/>
+      <c r="M1" s="107"/>
+      <c r="N1" s="107"/>
+      <c r="O1" s="107"/>
+      <c r="P1" s="107"/>
+      <c r="Q1" s="107"/>
+      <c r="R1" s="107"/>
+      <c r="S1" s="107"/>
+      <c r="T1" s="107"/>
+      <c r="U1" s="107"/>
+      <c r="V1" s="107"/>
+      <c r="W1" s="107"/>
+      <c r="X1" s="107"/>
+      <c r="Y1" s="107"/>
+      <c r="Z1" s="107"/>
+      <c r="AA1" s="107"/>
+      <c r="AB1" s="107"/>
+      <c r="AC1" s="107"/>
+      <c r="AD1" s="108"/>
     </row>
     <row r="2" spans="1:30" ht="10.5" customHeight="1">
-      <c r="A2" s="166"/>
-      <c r="B2" s="169"/>
-      <c r="C2" s="173"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="178"/>
-      <c r="F2" s="180"/>
+      <c r="A2" s="110"/>
+      <c r="B2" s="113"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="124"/>
       <c r="G2" s="46">
         <v>22</v>
       </c>
@@ -6492,12 +6492,12 @@
       </c>
     </row>
     <row r="3" spans="1:30" s="2" customFormat="1" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A3" s="167"/>
-      <c r="B3" s="170"/>
-      <c r="C3" s="175"/>
-      <c r="D3" s="176"/>
-      <c r="E3" s="182"/>
-      <c r="F3" s="181"/>
+      <c r="A3" s="111"/>
+      <c r="B3" s="114"/>
+      <c r="C3" s="119"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="206"/>
+      <c r="F3" s="125"/>
       <c r="G3" s="48" t="s">
         <v>18</v>
       </c>
@@ -6572,20 +6572,20 @@
       </c>
     </row>
     <row r="4" spans="1:30" ht="13.5" customHeight="1">
-      <c r="A4" s="157">
+      <c r="A4" s="126">
         <v>1</v>
       </c>
       <c r="B4" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="158" t="s">
+      <c r="C4" s="128" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="159"/>
-      <c r="E4" s="188" t="s">
+      <c r="D4" s="129"/>
+      <c r="E4" s="200" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="160"/>
+      <c r="F4" s="134"/>
       <c r="G4" s="49"/>
       <c r="H4" s="29"/>
       <c r="I4" s="29"/>
@@ -6608,20 +6608,20 @@
       <c r="Z4" s="12"/>
       <c r="AA4" s="18"/>
       <c r="AB4" s="10"/>
-      <c r="AC4" s="190" t="s">
+      <c r="AC4" s="202" t="s">
         <v>14</v>
       </c>
-      <c r="AD4" s="183" t="s">
+      <c r="AD4" s="195" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="13.5" customHeight="1">
-      <c r="A5" s="131"/>
+      <c r="A5" s="127"/>
       <c r="B5" s="34"/>
-      <c r="C5" s="111"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="189"/>
-      <c r="F5" s="161"/>
+      <c r="C5" s="130"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="201"/>
+      <c r="F5" s="135"/>
       <c r="G5" s="50"/>
       <c r="H5" s="31"/>
       <c r="I5" s="9"/>
@@ -6644,22 +6644,22 @@
       <c r="Z5" s="16"/>
       <c r="AA5" s="22"/>
       <c r="AB5" s="9"/>
-      <c r="AC5" s="191"/>
-      <c r="AD5" s="184"/>
+      <c r="AC5" s="203"/>
+      <c r="AD5" s="196"/>
     </row>
     <row r="6" spans="1:30" ht="13.5" customHeight="1">
-      <c r="A6" s="130">
+      <c r="A6" s="136">
         <v>2</v>
       </c>
       <c r="B6" s="34"/>
-      <c r="C6" s="128" t="s">
+      <c r="C6" s="143" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="129"/>
-      <c r="E6" s="186" t="s">
+      <c r="D6" s="144"/>
+      <c r="E6" s="198" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="155"/>
+      <c r="F6" s="148"/>
       <c r="G6" s="51"/>
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
@@ -6682,16 +6682,16 @@
       <c r="Z6" s="13"/>
       <c r="AA6" s="19"/>
       <c r="AB6" s="7"/>
-      <c r="AC6" s="191"/>
-      <c r="AD6" s="184"/>
+      <c r="AC6" s="203"/>
+      <c r="AD6" s="196"/>
     </row>
     <row r="7" spans="1:30" ht="13.5" customHeight="1">
-      <c r="A7" s="131"/>
+      <c r="A7" s="127"/>
       <c r="B7" s="34"/>
-      <c r="C7" s="132"/>
-      <c r="D7" s="133"/>
-      <c r="E7" s="187"/>
-      <c r="F7" s="156"/>
+      <c r="C7" s="145"/>
+      <c r="D7" s="146"/>
+      <c r="E7" s="199"/>
+      <c r="F7" s="149"/>
       <c r="G7" s="52"/>
       <c r="H7" s="32"/>
       <c r="I7" s="24"/>
@@ -6714,24 +6714,24 @@
       <c r="Z7" s="25"/>
       <c r="AA7" s="26"/>
       <c r="AB7" s="24"/>
-      <c r="AC7" s="191"/>
-      <c r="AD7" s="184"/>
+      <c r="AC7" s="203"/>
+      <c r="AD7" s="196"/>
     </row>
     <row r="8" spans="1:30" ht="13.5" customHeight="1">
-      <c r="A8" s="193">
+      <c r="A8" s="184">
         <v>3</v>
       </c>
       <c r="B8" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="113" t="s">
+      <c r="C8" s="176" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="114"/>
-      <c r="E8" s="195" t="s">
+      <c r="D8" s="177"/>
+      <c r="E8" s="205" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="150"/>
+      <c r="F8" s="155"/>
       <c r="G8" s="38"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -6754,16 +6754,16 @@
       <c r="Z8" s="15"/>
       <c r="AA8" s="21"/>
       <c r="AB8" s="6"/>
-      <c r="AC8" s="191"/>
-      <c r="AD8" s="184"/>
+      <c r="AC8" s="203"/>
+      <c r="AD8" s="196"/>
     </row>
     <row r="9" spans="1:30" ht="13.5" customHeight="1">
-      <c r="A9" s="194"/>
+      <c r="A9" s="185"/>
       <c r="B9" s="37"/>
-      <c r="C9" s="119"/>
-      <c r="D9" s="120"/>
-      <c r="E9" s="196"/>
-      <c r="F9" s="153"/>
+      <c r="C9" s="178"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="190"/>
+      <c r="F9" s="158"/>
       <c r="G9" s="53"/>
       <c r="H9" s="43"/>
       <c r="I9" s="43"/>
@@ -6786,24 +6786,24 @@
       <c r="Z9" s="44"/>
       <c r="AA9" s="45"/>
       <c r="AB9" s="43"/>
-      <c r="AC9" s="191"/>
-      <c r="AD9" s="184"/>
+      <c r="AC9" s="203"/>
+      <c r="AD9" s="196"/>
     </row>
     <row r="10" spans="1:30" ht="12" customHeight="1">
-      <c r="A10" s="197">
+      <c r="A10" s="193">
         <v>4</v>
       </c>
       <c r="B10" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="117" t="s">
+      <c r="C10" s="137" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="118"/>
-      <c r="E10" s="198" t="s">
+      <c r="D10" s="138"/>
+      <c r="E10" s="192" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="154"/>
+      <c r="F10" s="141"/>
       <c r="G10" s="50"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
@@ -6826,16 +6826,16 @@
       <c r="Z10" s="16"/>
       <c r="AA10" s="22"/>
       <c r="AB10" s="9"/>
-      <c r="AC10" s="191"/>
-      <c r="AD10" s="184"/>
+      <c r="AC10" s="203"/>
+      <c r="AD10" s="196"/>
     </row>
     <row r="11" spans="1:30" ht="12" customHeight="1">
-      <c r="A11" s="194"/>
+      <c r="A11" s="185"/>
       <c r="B11" s="36"/>
-      <c r="C11" s="115"/>
-      <c r="D11" s="116"/>
-      <c r="E11" s="199"/>
-      <c r="F11" s="151"/>
+      <c r="C11" s="139"/>
+      <c r="D11" s="140"/>
+      <c r="E11" s="188"/>
+      <c r="F11" s="142"/>
       <c r="G11" s="50"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
@@ -6858,19 +6858,19 @@
       <c r="Z11" s="16"/>
       <c r="AA11" s="22"/>
       <c r="AB11" s="9"/>
-      <c r="AC11" s="191"/>
-      <c r="AD11" s="184"/>
+      <c r="AC11" s="203"/>
+      <c r="AD11" s="196"/>
     </row>
     <row r="12" spans="1:30" ht="12" customHeight="1">
-      <c r="A12" s="193">
+      <c r="A12" s="184">
         <v>5</v>
       </c>
       <c r="B12" s="36"/>
-      <c r="C12" s="128" t="s">
+      <c r="C12" s="143" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="129"/>
-      <c r="E12" s="200" t="s">
+      <c r="D12" s="144"/>
+      <c r="E12" s="194" t="s">
         <v>37</v>
       </c>
       <c r="F12" s="152"/>
@@ -6896,16 +6896,16 @@
       <c r="Z12" s="13"/>
       <c r="AA12" s="19"/>
       <c r="AB12" s="7"/>
-      <c r="AC12" s="191"/>
-      <c r="AD12" s="184"/>
+      <c r="AC12" s="203"/>
+      <c r="AD12" s="196"/>
     </row>
     <row r="13" spans="1:30" ht="12" customHeight="1">
-      <c r="A13" s="197"/>
+      <c r="A13" s="193"/>
       <c r="B13" s="36"/>
-      <c r="C13" s="109"/>
-      <c r="D13" s="110"/>
-      <c r="E13" s="198"/>
-      <c r="F13" s="154"/>
+      <c r="C13" s="150"/>
+      <c r="D13" s="151"/>
+      <c r="E13" s="192"/>
+      <c r="F13" s="141"/>
       <c r="G13" s="52"/>
       <c r="H13" s="24"/>
       <c r="I13" s="24"/>
@@ -6928,24 +6928,24 @@
       <c r="Z13" s="25"/>
       <c r="AA13" s="26"/>
       <c r="AB13" s="24"/>
-      <c r="AC13" s="191"/>
-      <c r="AD13" s="184"/>
+      <c r="AC13" s="203"/>
+      <c r="AD13" s="196"/>
     </row>
     <row r="14" spans="1:30" ht="12" customHeight="1">
-      <c r="A14" s="201">
+      <c r="A14" s="189">
         <v>6</v>
       </c>
       <c r="B14" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="137" t="s">
+      <c r="C14" s="153" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="138"/>
-      <c r="E14" s="202" t="s">
+      <c r="D14" s="154"/>
+      <c r="E14" s="191" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="150"/>
+      <c r="F14" s="155"/>
       <c r="G14" s="38"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
@@ -6968,16 +6968,16 @@
       <c r="Z14" s="15"/>
       <c r="AA14" s="21"/>
       <c r="AB14" s="6"/>
-      <c r="AC14" s="191"/>
-      <c r="AD14" s="184"/>
+      <c r="AC14" s="203"/>
+      <c r="AD14" s="196"/>
     </row>
     <row r="15" spans="1:30" ht="12" customHeight="1">
-      <c r="A15" s="201"/>
+      <c r="A15" s="189"/>
       <c r="B15" s="36"/>
-      <c r="C15" s="111"/>
-      <c r="D15" s="112"/>
-      <c r="E15" s="199"/>
-      <c r="F15" s="151"/>
+      <c r="C15" s="130"/>
+      <c r="D15" s="131"/>
+      <c r="E15" s="188"/>
+      <c r="F15" s="142"/>
       <c r="G15" s="52"/>
       <c r="H15" s="24"/>
       <c r="I15" s="24"/>
@@ -7000,19 +7000,19 @@
       <c r="Z15" s="25"/>
       <c r="AA15" s="26"/>
       <c r="AB15" s="24"/>
-      <c r="AC15" s="191"/>
-      <c r="AD15" s="184"/>
+      <c r="AC15" s="203"/>
+      <c r="AD15" s="196"/>
     </row>
     <row r="16" spans="1:30" ht="12" customHeight="1">
-      <c r="A16" s="201">
+      <c r="A16" s="189">
         <v>7</v>
       </c>
       <c r="B16" s="36"/>
-      <c r="C16" s="128" t="s">
+      <c r="C16" s="143" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="129"/>
-      <c r="E16" s="203" t="s">
+      <c r="D16" s="144"/>
+      <c r="E16" s="187" t="s">
         <v>39</v>
       </c>
       <c r="F16" s="152"/>
@@ -7038,16 +7038,16 @@
       <c r="Z16" s="13"/>
       <c r="AA16" s="19"/>
       <c r="AB16" s="7"/>
-      <c r="AC16" s="191"/>
-      <c r="AD16" s="184"/>
+      <c r="AC16" s="203"/>
+      <c r="AD16" s="196"/>
     </row>
     <row r="17" spans="1:30" ht="12" customHeight="1">
-      <c r="A17" s="201"/>
+      <c r="A17" s="189"/>
       <c r="B17" s="36"/>
-      <c r="C17" s="111"/>
-      <c r="D17" s="112"/>
-      <c r="E17" s="199"/>
-      <c r="F17" s="151"/>
+      <c r="C17" s="130"/>
+      <c r="D17" s="131"/>
+      <c r="E17" s="188"/>
+      <c r="F17" s="142"/>
       <c r="G17" s="52"/>
       <c r="H17" s="24"/>
       <c r="I17" s="24"/>
@@ -7070,19 +7070,19 @@
       <c r="Z17" s="25"/>
       <c r="AA17" s="26"/>
       <c r="AB17" s="24"/>
-      <c r="AC17" s="191"/>
-      <c r="AD17" s="184"/>
+      <c r="AC17" s="203"/>
+      <c r="AD17" s="196"/>
     </row>
     <row r="18" spans="1:30" ht="12" customHeight="1">
-      <c r="A18" s="201">
+      <c r="A18" s="189">
         <v>8</v>
       </c>
       <c r="B18" s="36"/>
-      <c r="C18" s="128" t="s">
+      <c r="C18" s="143" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="129"/>
-      <c r="E18" s="203" t="s">
+      <c r="D18" s="144"/>
+      <c r="E18" s="187" t="s">
         <v>40</v>
       </c>
       <c r="F18" s="152"/>
@@ -7108,16 +7108,16 @@
       <c r="Z18" s="25"/>
       <c r="AA18" s="26"/>
       <c r="AB18" s="24"/>
-      <c r="AC18" s="191"/>
-      <c r="AD18" s="184"/>
+      <c r="AC18" s="203"/>
+      <c r="AD18" s="196"/>
     </row>
     <row r="19" spans="1:30" ht="12" customHeight="1">
-      <c r="A19" s="201"/>
+      <c r="A19" s="189"/>
       <c r="B19" s="37"/>
-      <c r="C19" s="132"/>
-      <c r="D19" s="133"/>
-      <c r="E19" s="196"/>
-      <c r="F19" s="153"/>
+      <c r="C19" s="145"/>
+      <c r="D19" s="146"/>
+      <c r="E19" s="190"/>
+      <c r="F19" s="158"/>
       <c r="G19" s="54"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
@@ -7140,24 +7140,24 @@
       <c r="Z19" s="17"/>
       <c r="AA19" s="23"/>
       <c r="AB19" s="8"/>
-      <c r="AC19" s="191"/>
-      <c r="AD19" s="184"/>
+      <c r="AC19" s="203"/>
+      <c r="AD19" s="196"/>
     </row>
     <row r="20" spans="1:30" ht="12" customHeight="1">
-      <c r="A20" s="193">
+      <c r="A20" s="184">
         <v>9</v>
       </c>
       <c r="B20" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="137" t="s">
+      <c r="C20" s="153" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="138"/>
-      <c r="E20" s="202" t="s">
+      <c r="D20" s="154"/>
+      <c r="E20" s="191" t="s">
         <v>41</v>
       </c>
-      <c r="F20" s="150"/>
+      <c r="F20" s="155"/>
       <c r="G20" s="38"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
@@ -7180,18 +7180,18 @@
       <c r="Z20" s="15"/>
       <c r="AA20" s="21"/>
       <c r="AB20" s="6"/>
-      <c r="AC20" s="191"/>
-      <c r="AD20" s="184"/>
+      <c r="AC20" s="203"/>
+      <c r="AD20" s="196"/>
     </row>
     <row r="21" spans="1:30" ht="12" customHeight="1">
-      <c r="A21" s="194"/>
+      <c r="A21" s="185"/>
       <c r="B21" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="111"/>
-      <c r="D21" s="112"/>
-      <c r="E21" s="199"/>
-      <c r="F21" s="151"/>
+      <c r="C21" s="130"/>
+      <c r="D21" s="131"/>
+      <c r="E21" s="188"/>
+      <c r="F21" s="142"/>
       <c r="G21" s="51"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
@@ -7214,19 +7214,19 @@
       <c r="Z21" s="13"/>
       <c r="AA21" s="19"/>
       <c r="AB21" s="7"/>
-      <c r="AC21" s="191"/>
-      <c r="AD21" s="184"/>
+      <c r="AC21" s="203"/>
+      <c r="AD21" s="196"/>
     </row>
     <row r="22" spans="1:30" ht="12" customHeight="1">
-      <c r="A22" s="193">
+      <c r="A22" s="184">
         <v>10</v>
       </c>
       <c r="B22" s="36"/>
-      <c r="C22" s="204" t="s">
+      <c r="C22" s="186" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="129"/>
-      <c r="E22" s="203" t="s">
+      <c r="D22" s="144"/>
+      <c r="E22" s="187" t="s">
         <v>42</v>
       </c>
       <c r="F22" s="152"/>
@@ -7252,16 +7252,16 @@
       <c r="Z22" s="13"/>
       <c r="AA22" s="19"/>
       <c r="AB22" s="7"/>
-      <c r="AC22" s="191"/>
-      <c r="AD22" s="184"/>
+      <c r="AC22" s="203"/>
+      <c r="AD22" s="196"/>
     </row>
     <row r="23" spans="1:30" ht="12" customHeight="1">
-      <c r="A23" s="194"/>
+      <c r="A23" s="185"/>
       <c r="B23" s="36"/>
-      <c r="C23" s="111"/>
-      <c r="D23" s="112"/>
-      <c r="E23" s="199"/>
-      <c r="F23" s="151"/>
+      <c r="C23" s="130"/>
+      <c r="D23" s="131"/>
+      <c r="E23" s="188"/>
+      <c r="F23" s="142"/>
       <c r="G23" s="51"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
@@ -7284,19 +7284,19 @@
       <c r="Z23" s="13"/>
       <c r="AA23" s="19"/>
       <c r="AB23" s="7"/>
-      <c r="AC23" s="191"/>
-      <c r="AD23" s="184"/>
+      <c r="AC23" s="203"/>
+      <c r="AD23" s="196"/>
     </row>
     <row r="24" spans="1:30" ht="12" customHeight="1">
-      <c r="A24" s="193">
+      <c r="A24" s="184">
         <v>11</v>
       </c>
       <c r="B24" s="36"/>
-      <c r="C24" s="204" t="s">
+      <c r="C24" s="186" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="129"/>
-      <c r="E24" s="203" t="s">
+      <c r="D24" s="144"/>
+      <c r="E24" s="187" t="s">
         <v>43</v>
       </c>
       <c r="F24" s="152"/>
@@ -7322,16 +7322,16 @@
       <c r="Z24" s="25"/>
       <c r="AA24" s="26"/>
       <c r="AB24" s="24"/>
-      <c r="AC24" s="191"/>
-      <c r="AD24" s="184"/>
+      <c r="AC24" s="203"/>
+      <c r="AD24" s="196"/>
     </row>
     <row r="25" spans="1:30" ht="12" customHeight="1">
-      <c r="A25" s="194"/>
+      <c r="A25" s="185"/>
       <c r="B25" s="37"/>
-      <c r="C25" s="111"/>
-      <c r="D25" s="112"/>
-      <c r="E25" s="199"/>
-      <c r="F25" s="153"/>
+      <c r="C25" s="130"/>
+      <c r="D25" s="131"/>
+      <c r="E25" s="188"/>
+      <c r="F25" s="158"/>
       <c r="G25" s="54"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
@@ -7354,24 +7354,24 @@
       <c r="Z25" s="17"/>
       <c r="AA25" s="23"/>
       <c r="AB25" s="8"/>
-      <c r="AC25" s="191"/>
-      <c r="AD25" s="184"/>
+      <c r="AC25" s="203"/>
+      <c r="AD25" s="196"/>
     </row>
     <row r="26" spans="1:30" ht="12" customHeight="1">
-      <c r="A26" s="130">
+      <c r="A26" s="136">
         <v>12</v>
       </c>
       <c r="B26" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="144" t="s">
+      <c r="C26" s="159" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="145"/>
-      <c r="E26" s="205" t="s">
+      <c r="D26" s="160"/>
+      <c r="E26" s="182" t="s">
         <v>35</v>
       </c>
-      <c r="F26" s="148"/>
+      <c r="F26" s="163"/>
       <c r="G26" s="38"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
@@ -7394,16 +7394,16 @@
       <c r="Z26" s="15"/>
       <c r="AA26" s="21"/>
       <c r="AB26" s="6"/>
-      <c r="AC26" s="191"/>
-      <c r="AD26" s="184"/>
+      <c r="AC26" s="203"/>
+      <c r="AD26" s="196"/>
     </row>
     <row r="27" spans="1:30" ht="12" customHeight="1">
-      <c r="A27" s="131"/>
+      <c r="A27" s="127"/>
       <c r="B27" s="34"/>
-      <c r="C27" s="146"/>
-      <c r="D27" s="147"/>
-      <c r="E27" s="206"/>
-      <c r="F27" s="149"/>
+      <c r="C27" s="161"/>
+      <c r="D27" s="162"/>
+      <c r="E27" s="183"/>
+      <c r="F27" s="164"/>
       <c r="G27" s="51"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
@@ -7426,24 +7426,24 @@
       <c r="Z27" s="13"/>
       <c r="AA27" s="19"/>
       <c r="AB27" s="7"/>
-      <c r="AC27" s="191"/>
-      <c r="AD27" s="184"/>
+      <c r="AC27" s="203"/>
+      <c r="AD27" s="196"/>
     </row>
     <row r="28" spans="1:30" ht="12" customHeight="1">
-      <c r="A28" s="130">
+      <c r="A28" s="136">
         <v>14</v>
       </c>
-      <c r="B28" s="135" t="s">
+      <c r="B28" s="168" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="137" t="s">
+      <c r="C28" s="153" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="138"/>
-      <c r="E28" s="135" t="s">
+      <c r="D28" s="154"/>
+      <c r="E28" s="168" t="s">
         <v>35</v>
       </c>
-      <c r="F28" s="142"/>
+      <c r="F28" s="173"/>
       <c r="G28" s="38"/>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
@@ -7466,16 +7466,16 @@
       <c r="Z28" s="15"/>
       <c r="AA28" s="21"/>
       <c r="AB28" s="40"/>
-      <c r="AC28" s="191"/>
-      <c r="AD28" s="184"/>
+      <c r="AC28" s="203"/>
+      <c r="AD28" s="196"/>
     </row>
     <row r="29" spans="1:30" ht="12" customHeight="1" thickBot="1">
-      <c r="A29" s="134"/>
-      <c r="B29" s="136"/>
-      <c r="C29" s="139"/>
-      <c r="D29" s="140"/>
-      <c r="E29" s="136"/>
-      <c r="F29" s="143"/>
+      <c r="A29" s="167"/>
+      <c r="B29" s="169"/>
+      <c r="C29" s="170"/>
+      <c r="D29" s="171"/>
+      <c r="E29" s="169"/>
+      <c r="F29" s="174"/>
       <c r="G29" s="39"/>
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
@@ -7498,8 +7498,8 @@
       <c r="Z29" s="14"/>
       <c r="AA29" s="20"/>
       <c r="AB29" s="11"/>
-      <c r="AC29" s="192"/>
-      <c r="AD29" s="185"/>
+      <c r="AC29" s="204"/>
+      <c r="AD29" s="197"/>
     </row>
     <row r="30" spans="1:30">
       <c r="Z30" s="5"/>
@@ -7519,45 +7519,12 @@
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="C26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="C22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="C24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="C20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="C14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="C16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="C12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G1:AD1"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
     <mergeCell ref="AD4:AD29"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="C6:D7"/>
@@ -7574,12 +7541,45 @@
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="C10:D11"/>
-    <mergeCell ref="G1:AD1"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="C12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="C14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="C16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="C20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="C22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="C24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="C26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <printOptions gridLinesSet="0"/>

</xml_diff>